<commit_message>
What's Today's Menu - 2814874440 업데이트
</commit_message>
<xml_diff>
--- a/Pull Request Here/What's Today's Menu - 2814874440/What's Today's Menu - 2814874440.xlsx
+++ b/Pull Request Here/What's Today's Menu - 2814874440/What's Today's Menu - 2814874440.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\What's Today's Menu - 2814874440\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C9686A-FEE5-4605-AC11-EF802DB78A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22E77EE-CCD6-4D6E-998D-E71EE782406A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="390">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -730,601 +730,610 @@
     <t>Keyed</t>
   </si>
   <si>
+    <t>Keyed+meat</t>
+  </si>
+  <si>
+    <t>meat</t>
+  </si>
+  <si>
+    <t>Keyed+meatPost</t>
+  </si>
+  <si>
+    <t>meatPost</t>
+  </si>
+  <si>
+    <t>Keyed+cow</t>
+  </si>
+  <si>
+    <t>cow</t>
+  </si>
+  <si>
+    <t>Keyed+unfert</t>
+  </si>
+  <si>
+    <t>fert</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (fert.)</t>
+  </si>
+  <si>
+    <t>꾸이 차타도</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>omelette</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>햄버거</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient yogurt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 요거트</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient bowl</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>콩조림 토스트</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>warm salad of boiled peas</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>corn flakes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 로코모코</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>beans on toast</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>corn pottage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>옥수수 포타주</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 데리야끼</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 크림 스튜</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>클램차우더</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 스튜</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>김치볶음밥</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>칠리 콘 카르네</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>마파두부</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 타르트</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>coleslaw</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>피시 앤 칩스</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient quiche</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>코울슬로</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>borscht</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>보르시</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 수프</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tofu</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 양갱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>두부조림</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fried egg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheese</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>치즈스틱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>야채 스튜</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient BBQ skewers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>donner kebab</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>되네르 케밥</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>swedish meatballs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>가츠동</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>코코뱅</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>lasagna</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chicken dinner</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient cake</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 케이크</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>치즈 크러스트 피자</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient steak set meal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 스테이크 정식</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 스트로가노프</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>타코 바르바코아</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 초밥</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 모찌</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient mochi</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WTM_FruitMochi.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tomato spagetti</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>토마토 스파게티</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>까르보나라</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>투움바 파스타</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 파이</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 스테이크</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>치즈 리조또</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient pancake</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>우유죽</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>폴렌타</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient smoothie</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ancient cheese</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>핫 크리스피 치킨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>왕돈까스</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>치즈</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>삶은 /ingredient</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WhatsTodaysMenu.MenuPatternDef</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simple</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lavish</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fine</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient국</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrapped grilled /ingredient</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회오리 감자</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>마약 옥수수</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>궁중 떡볶이</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 바베큐</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient튀김 정식</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>숯불 /ingredient말이</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 리소토</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>버터 알감자</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>구운 /ingredient</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient구이</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>계란찜</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>베스킨라빈스</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 꼬치</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient parfait</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 파르페</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>steak with /ingredient sause</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WTM_SteakBerry.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient소스 스테이크</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WTM_SearedFish.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>seared /ingredient steak</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수비드 /ingredient 스테이크</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>meat loaf</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>떡갈비</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 오마카세</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>트러플 머쉬룸 파스타</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>오니기리</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>꽃빵</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>티라미수</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>스크램블 에그덮밥</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>프렌치 오믈렛</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>어니언 수프</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>배추겉절이</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WTM_FishPancake.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chili /ingredient</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WTM_FishChili.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>미트볼</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WTM_PeasSalad.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>칠리/ingredient</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 시저 샐러드</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 사라다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 와플</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>샤슐릭</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>polenta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient비빔밥</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient해물파전</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient볶음</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keyed+fert</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keyed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>추출 툴로 안나옵니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(작성안해도 됨)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>beef</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cowPost</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>unfert</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient잼 토스트</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>웨지 포테이토</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>콘플레이크</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>완두콩 포케</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>raw</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> meat</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> (unfert.)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">raw </t>
-  </si>
-  <si>
-    <t>Keyed+meat</t>
-  </si>
-  <si>
-    <t>meat</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> meat</t>
-  </si>
-  <si>
-    <t>Keyed+meatPost</t>
-  </si>
-  <si>
-    <t>meatPost</t>
-  </si>
-  <si>
-    <t>Keyed+cow</t>
-  </si>
-  <si>
-    <t>cow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Keyed+cowPost</t>
-  </si>
-  <si>
-    <t>Keyed+unfert</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (unfert.)</t>
-  </si>
-  <si>
-    <t>fert</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (fert.)</t>
-  </si>
-  <si>
-    <t>꾸이 차타도</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>omelette</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>햄버거</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient yogurt</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 요거트</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 잼 토스트</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient bowl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>콩조림 토스트</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>warm salad of boiled peas</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>corn flakes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 로코모코</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>beans on toast</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>corn pottage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>옥수수 포타주</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 데리야끼</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 크림 스튜</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>클램차우더</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 스튜</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>김치볶음밥</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>칠리 콘 카르네</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>마파두부</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 타르트</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>coleslaw</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>피시 앤 칩스</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient quiche</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>코울슬로</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>borscht</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>보르시</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 수프</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tofu</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 양갱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>두부조림</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fried egg</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cheese</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>치즈스틱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>야채 스튜</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient BBQ skewers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>donner kebab</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>되네르 케밥</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>swedish meatballs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>가츠동</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>코코뱅</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>lasagna</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chicken dinner</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient cake</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 케이크</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>치즈 크러스트 피자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient steak set meal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 스테이크 정식</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 스트로가노프</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>타코 바르바코아</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 초밥</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 모찌</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient mochi</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WTM_FruitMochi.label</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tomato spagetti</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>토마토 스파게티</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>까르보나라</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>투움바 파스타</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 파이</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 스테이크</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>치즈 리조또</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient pancake</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>죽</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>우유죽</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>폴렌타</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient smoothie</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ancient cheese</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>웨지 감자튀김</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>핫 크리스피 치킨</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>왕돈까스</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>치즈</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>삶은 /ingredient</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WhatsTodaysMenu.MenuPatternDef</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Simple</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lavish</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fine</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient국</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>wrapped grilled /ingredient</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회오리 감자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>마약 옥수수</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>궁중 떡볶이</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>콘치즈</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 바베큐</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient튀김 정식</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>숯불 /ingredient말이</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 리소토</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>버터 알감자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>구운 /ingredient</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient구이</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>계란찜</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>베스킨라빈스</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 꼬치</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient parfait</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 파르페</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>steak with /ingredient sause</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WTM_SteakBerry.label</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient소스 스테이크</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WTM_SearedFish.label</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>seared /ingredient steak</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수비드 /ingredient 스테이크</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>meat loaf</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>떡갈비</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 오마카세</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>트러플 머쉬룸 파스타</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>오니기리</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>꽃빵</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>티라미수</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>스크램블 에그덮밥</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>프렌치 오믈렛</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>어니언 수프</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>배추겉절이</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WTM_FishPancake.label</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chili /ingredient</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WTM_FishChili.label</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>미트볼</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WTM_PeasSalad.label</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>칠리/ingredient</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>웜 샐러드</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 시저 샐러드</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 사라다</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient 와플</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>샤슐릭</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>polenta</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient비빔밥</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient해물파전</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/ingredient볶음</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Keyed+fert</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Keyed+groundMeat</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ground meat</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Keyed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>추출 툴로 안나옵니다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(작성안해도 됨)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>beef</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>groundMeat</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cowPost</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>unfert</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>특제 양념</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WhatsTodaysMenu.IngredientCategoryDef+WTMCategory_MeatGroundable.duplicatedLabel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patches.WhatsTodaysMenu.IngredientCategoryDef</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WTMCategory_MeatGroundable.duplicatedLabel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ground meat</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>함박</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1378,12 +1387,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1397,6 +1400,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1426,7 +1435,7 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1438,21 +1447,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="메모" xfId="1" builtinId="10"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
@@ -1802,10 +1812,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1822,7 +1832,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1836,10 +1846,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1856,7 +1866,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1870,10 +1880,10 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1890,7 +1900,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1907,7 +1917,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1924,7 +1934,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>255</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1938,10 +1948,10 @@
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1955,10 +1965,10 @@
         <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1969,13 +1979,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1989,10 +1999,10 @@
         <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>332</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2006,10 +2016,10 @@
         <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2026,7 +2036,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2043,7 +2053,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>318</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2060,7 +2070,7 @@
         <v>46</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2077,7 +2087,7 @@
         <v>49</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2088,13 +2098,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2105,13 +2115,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2128,7 +2138,7 @@
         <v>54</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2145,7 +2155,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2162,7 +2172,7 @@
         <v>60</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2179,7 +2189,7 @@
         <v>63</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2196,7 +2206,7 @@
         <v>63</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2213,7 +2223,7 @@
         <v>68</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -2230,7 +2240,7 @@
         <v>71</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2247,7 +2257,7 @@
         <v>74</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2261,10 +2271,10 @@
         <v>76</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2278,10 +2288,10 @@
         <v>78</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2295,10 +2305,10 @@
         <v>80</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2315,7 +2325,7 @@
         <v>83</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2332,7 +2342,7 @@
         <v>86</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2346,10 +2356,10 @@
         <v>88</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2366,7 +2376,7 @@
         <v>91</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2383,7 +2393,7 @@
         <v>94</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2400,7 +2410,7 @@
         <v>97</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2414,10 +2424,10 @@
         <v>99</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2431,10 +2441,10 @@
         <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2448,10 +2458,10 @@
         <v>103</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2468,7 +2478,7 @@
         <v>106</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2482,10 +2492,10 @@
         <v>108</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2499,10 +2509,10 @@
         <v>110</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2516,10 +2526,10 @@
         <v>112</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2535,11 +2545,11 @@
       <c r="E45" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>325</v>
+      <c r="F45" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2555,8 +2565,8 @@
       <c r="E46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>320</v>
+      <c r="F46" s="10" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2572,8 +2582,8 @@
       <c r="E47" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>291</v>
+      <c r="F47" s="10" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2587,10 +2597,10 @@
         <v>123</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>319</v>
+        <v>287</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2604,10 +2614,10 @@
         <v>125</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>354</v>
+        <v>286</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2621,10 +2631,10 @@
         <v>127</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2640,8 +2650,8 @@
       <c r="E51" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F51" s="4" t="s">
-        <v>296</v>
+      <c r="F51" s="10" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2655,10 +2665,10 @@
         <v>132</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>298</v>
+        <v>291</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2674,8 +2684,8 @@
       <c r="E53" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>299</v>
+      <c r="F53" s="10" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2691,8 +2701,8 @@
       <c r="E54" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>300</v>
+      <c r="F54" s="10" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2708,8 +2718,8 @@
       <c r="E55" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>301</v>
+      <c r="F55" s="10" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2720,13 +2730,13 @@
         <v>7</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2740,10 +2750,10 @@
         <v>144</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>306</v>
+        <v>299</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2759,8 +2769,8 @@
       <c r="E58" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>307</v>
+      <c r="F58" s="10" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2776,8 +2786,8 @@
       <c r="E59" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>308</v>
+      <c r="F59" s="10" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2793,8 +2803,8 @@
       <c r="E60" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>309</v>
+      <c r="F60" s="10" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2810,8 +2820,8 @@
       <c r="E61" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>371</v>
+      <c r="F61" s="10" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2825,10 +2835,10 @@
         <v>157</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>344</v>
+        <v>335</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2844,8 +2854,8 @@
       <c r="E63" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>310</v>
+      <c r="F63" s="10" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2859,10 +2869,10 @@
         <v>162</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>352</v>
+        <v>343</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2873,13 +2883,13 @@
         <v>7</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>347</v>
+        <v>337</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2890,13 +2900,13 @@
         <v>7</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>350</v>
+        <v>341</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2912,8 +2922,8 @@
       <c r="E67" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F67" s="4" t="s">
-        <v>353</v>
+      <c r="F67" s="10" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2921,7 +2931,7 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>169</v>
@@ -2929,8 +2939,8 @@
       <c r="E68" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F68" s="4" t="s">
-        <v>331</v>
+      <c r="F68" s="10" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2946,8 +2956,8 @@
       <c r="E69" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F69" s="4" t="s">
-        <v>330</v>
+      <c r="F69" s="10" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2963,8 +2973,8 @@
       <c r="E70" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F70" s="4" t="s">
-        <v>329</v>
+      <c r="F70" s="10" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2980,8 +2990,8 @@
       <c r="E71" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F71" s="4" t="s">
-        <v>341</v>
+      <c r="F71" s="10" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -2997,8 +3007,8 @@
       <c r="E72" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>357</v>
+      <c r="F72" s="10" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3014,8 +3024,8 @@
       <c r="E73" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F73" s="4" t="s">
-        <v>359</v>
+      <c r="F73" s="10" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3031,8 +3041,8 @@
       <c r="E74" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F74" s="4" t="s">
-        <v>370</v>
+      <c r="F74" s="10" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3048,8 +3058,8 @@
       <c r="E75" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F75" s="4" t="s">
-        <v>369</v>
+      <c r="F75" s="10" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3065,11 +3075,11 @@
       <c r="E76" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F76" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>324</v>
+      <c r="F76" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3085,8 +3095,8 @@
       <c r="E77" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F77" s="6" t="s">
-        <v>314</v>
+      <c r="F77" s="4" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3102,8 +3112,8 @@
       <c r="E78" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F78" s="6" t="s">
-        <v>336</v>
+      <c r="F78" s="4" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3117,10 +3127,10 @@
         <v>201</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>315</v>
+        <v>364</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3134,10 +3144,10 @@
         <v>203</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>342</v>
+        <v>310</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3151,10 +3161,10 @@
         <v>205</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>321</v>
+        <v>311</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3170,8 +3180,8 @@
       <c r="E82" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F82" s="6" t="s">
-        <v>322</v>
+      <c r="F82" s="4" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3187,8 +3197,8 @@
       <c r="E83" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F83" s="6" t="s">
-        <v>372</v>
+      <c r="F83" s="4" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3204,8 +3214,8 @@
       <c r="E84" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F84" s="6" t="s">
-        <v>327</v>
+      <c r="F84" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3221,8 +3231,8 @@
       <c r="E85" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="F85" s="6" t="s">
-        <v>338</v>
+      <c r="F85" s="4" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3238,8 +3248,8 @@
       <c r="E86" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F86" s="6" t="s">
-        <v>322</v>
+      <c r="F86" s="4" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3255,8 +3265,8 @@
       <c r="E87" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F87" s="6" t="s">
-        <v>327</v>
+      <c r="F87" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3272,8 +3282,8 @@
       <c r="E88" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F88" s="6" t="s">
-        <v>342</v>
+      <c r="F88" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3289,8 +3299,8 @@
       <c r="E89" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F89" s="6" t="s">
-        <v>327</v>
+      <c r="F89" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3306,8 +3316,8 @@
       <c r="E90" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F90" s="6" t="s">
-        <v>376</v>
+      <c r="F90" s="4" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3323,8 +3333,8 @@
       <c r="E91" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F91" s="6" t="s">
-        <v>327</v>
+      <c r="F91" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3340,8 +3350,8 @@
       <c r="E92" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F92" s="6" t="s">
-        <v>339</v>
+      <c r="F92" s="4" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3357,8 +3367,8 @@
       <c r="E93" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F93" s="6" t="s">
-        <v>327</v>
+      <c r="F93" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3369,121 +3379,121 @@
         <v>235</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>236</v>
+        <v>380</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F94" s="10"/>
-      <c r="G94" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="G94" s="6" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F95" s="10"/>
+        <v>381</v>
+      </c>
+      <c r="F95" s="8"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F96" s="10"/>
+        <v>239</v>
+      </c>
+      <c r="F96" s="8"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="F97" s="10"/>
+        <v>372</v>
+      </c>
+      <c r="F97" s="8"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>245</v>
+        <v>384</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="F98" s="10"/>
+        <v>373</v>
+      </c>
+      <c r="F98" s="8"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>235</v>
+        <v>369</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F99" s="10"/>
+        <v>382</v>
+      </c>
+      <c r="F99" s="8"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F100" s="10"/>
+        <v>244</v>
+      </c>
+      <c r="F100" s="8"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="F101" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="G101" s="9" t="s">
-        <v>381</v>
+      <c r="F101" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
What's Today's Menu 업데이트
</commit_message>
<xml_diff>
--- a/Pull Request Here/What's Today's Menu - 2814874440/What's Today's Menu - 2814874440.xlsx
+++ b/Pull Request Here/What's Today's Menu - 2814874440/What's Today's Menu - 2814874440.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22E77EE-CCD6-4D6E-998D-E71EE782406A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB1FF18-C1AA-4EF5-9412-FB931B3F163B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,10 +1033,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>치즈</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>삶은 /ingredient</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1334,6 +1330,10 @@
   </si>
   <si>
     <t>함박</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>생치즈</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1815,7 +1815,7 @@
         <v>254</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1849,7 +1849,7 @@
         <v>250</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1883,7 +1883,7 @@
         <v>246</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1900,7 +1900,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1934,7 +1934,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1979,13 +1979,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>252</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2002,7 +2002,7 @@
         <v>253</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2036,7 +2036,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2053,7 +2053,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2070,7 +2070,7 @@
         <v>46</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2098,13 +2098,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2115,13 +2115,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>306</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2271,10 +2271,10 @@
         <v>76</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2325,7 +2325,7 @@
         <v>83</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2342,7 +2342,7 @@
         <v>86</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2393,7 +2393,7 @@
         <v>94</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2444,7 +2444,7 @@
         <v>276</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2495,7 +2495,7 @@
         <v>280</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2529,7 +2529,7 @@
         <v>283</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2549,7 +2549,7 @@
         <v>284</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2617,7 +2617,7 @@
         <v>286</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2821,7 +2821,7 @@
         <v>153</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2835,10 +2835,10 @@
         <v>157</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>335</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2869,10 +2869,10 @@
         <v>162</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="F64" s="10" t="s">
         <v>343</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2883,13 +2883,13 @@
         <v>7</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F65" s="10" t="s">
         <v>338</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2900,13 +2900,13 @@
         <v>7</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="F66" s="10" t="s">
         <v>341</v>
-      </c>
-      <c r="F66" s="10" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2923,7 +2923,7 @@
         <v>167</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2931,7 +2931,7 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>169</v>
@@ -2940,7 +2940,7 @@
         <v>170</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2957,7 +2957,7 @@
         <v>173</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2974,7 +2974,7 @@
         <v>176</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2991,7 +2991,7 @@
         <v>179</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3008,7 +3008,7 @@
         <v>182</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3025,7 +3025,7 @@
         <v>185</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3042,7 +3042,7 @@
         <v>188</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3059,7 +3059,7 @@
         <v>188</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3079,7 +3079,7 @@
         <v>307</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3113,7 +3113,7 @@
         <v>199</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3127,7 +3127,7 @@
         <v>201</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>309</v>
@@ -3147,7 +3147,7 @@
         <v>310</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3164,7 +3164,7 @@
         <v>311</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>314</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3181,7 +3181,7 @@
         <v>208</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3198,7 +3198,7 @@
         <v>211</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3215,7 +3215,7 @@
         <v>91</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3232,7 +3232,7 @@
         <v>216</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3249,7 +3249,7 @@
         <v>208</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3266,7 +3266,7 @@
         <v>91</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3283,7 +3283,7 @@
         <v>223</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3300,7 +3300,7 @@
         <v>91</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3317,7 +3317,7 @@
         <v>223</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3334,7 +3334,7 @@
         <v>91</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3351,7 +3351,7 @@
         <v>223</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3368,7 +3368,7 @@
         <v>91</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3379,14 +3379,14 @@
         <v>235</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F94" s="8"/>
       <c r="G94" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3400,7 +3400,7 @@
         <v>237</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F95" s="8"/>
     </row>
@@ -3427,22 +3427,22 @@
         <v>241</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F97" s="8"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F98" s="8"/>
     </row>
@@ -3451,22 +3451,22 @@
         <v>242</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F99" s="8"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>243</v>
@@ -3478,22 +3478,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="F101" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="F101" s="9" t="s">
-        <v>389</v>
-      </c>
       <c r="G101" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
What's Today's Menu 업데이투
</commit_message>
<xml_diff>
--- a/Pull Request Here/What's Today's Menu - 2814874440/What's Today's Menu - 2814874440.xlsx
+++ b/Pull Request Here/What's Today's Menu - 2814874440/What's Today's Menu - 2814874440.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5D7C19-9B7B-4A43-85D8-8B40C3D62F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38976B07-CAEE-459D-B001-C951D4F98E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="405">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -837,10 +837,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>/ingredient 타르트</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>coleslaw</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -865,10 +861,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>/ingredient 수프</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>tofu</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -889,10 +881,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>치즈스틱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>야채 스튜</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -917,10 +905,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>코코뱅</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>lasagna</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1149,10 +1133,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>떡갈비</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>/ingredient 오마카세</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1181,10 +1161,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>어니언 수프</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>배추겉절이</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1201,10 +1177,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>미트볼</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>WTM_PeasSalad.label</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1233,10 +1205,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>/ingredient비빔밥</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>/ingredient해물파전</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1289,10 +1257,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>완두콩 포케</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>raw</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1334,6 +1298,311 @@
   </si>
   <si>
     <t>WhatsTodaysMenu.IngredientCategoryDef</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>치즈 퐁듀</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 필라프</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Egg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Rice</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rice</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>콩비지찌개</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Peas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Egg</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Potato</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Milk</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Fish</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Pepper</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient 키슈</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>잼은 보존식품</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>스웨디시 미트볼</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>꼬꼬뱅</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chiken</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Chiken</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Onion</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Pig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Cabbage</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Fungus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Milk</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Bread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Milk</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>자우어는 발효식품</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Fish</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Bread(=Wheat)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀푀유나베</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Meat(Multi)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Rice</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Meat(Multi)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Veg(All)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루밍 어니언</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ingredient수프</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1341,7 +1610,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1363,6 +1632,21 @@
     <font>
       <sz val="8"/>
       <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -1440,7 +1724,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1453,6 +1737,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="메모" xfId="1" builtinId="10"/>
@@ -1815,7 +2101,7 @@
         <v>254</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1849,7 +2135,10 @@
         <v>250</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>364</v>
+        <v>382</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1866,7 +2155,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1883,7 +2172,10 @@
         <v>246</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1900,7 +2192,10 @@
         <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1934,7 +2229,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1979,13 +2274,16 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>252</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>378</v>
+        <v>385</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2002,7 +2300,7 @@
         <v>253</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2036,7 +2334,10 @@
         <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2053,10 +2354,10 @@
         <v>43</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -2070,10 +2371,10 @@
         <v>46</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -2087,10 +2388,10 @@
         <v>49</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2098,16 +2399,19 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -2115,16 +2419,19 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
@@ -2141,7 +2448,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -2158,7 +2465,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
@@ -2175,7 +2482,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
@@ -2192,7 +2499,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
@@ -2209,7 +2516,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -2226,7 +2533,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -2243,7 +2550,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -2260,7 +2567,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
@@ -2271,13 +2578,13 @@
         <v>76</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
@@ -2288,13 +2595,13 @@
         <v>78</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>79</v>
       </c>
@@ -2305,13 +2612,13 @@
         <v>80</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -2325,7 +2632,10 @@
         <v>83</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2342,7 +2652,7 @@
         <v>86</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>351</v>
+        <v>403</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2356,10 +2666,10 @@
         <v>88</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2376,7 +2686,7 @@
         <v>91</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2393,7 +2703,7 @@
         <v>94</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2410,7 +2720,10 @@
         <v>97</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2424,10 +2737,10 @@
         <v>99</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2441,10 +2754,10 @@
         <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2458,10 +2771,10 @@
         <v>103</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>278</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2478,7 +2791,7 @@
         <v>106</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2492,10 +2805,10 @@
         <v>108</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2509,10 +2822,10 @@
         <v>110</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2526,10 +2839,10 @@
         <v>112</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>356</v>
+        <v>391</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2546,10 +2859,10 @@
         <v>115</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2566,7 +2879,10 @@
         <v>118</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>313</v>
+        <v>309</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2583,7 +2899,10 @@
         <v>121</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>285</v>
+        <v>392</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2597,13 +2916,16 @@
         <v>123</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>124</v>
       </c>
@@ -2614,13 +2936,16 @@
         <v>125</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>126</v>
       </c>
@@ -2631,13 +2956,13 @@
         <v>127</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>128</v>
       </c>
@@ -2651,10 +2976,13 @@
         <v>130</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>131</v>
       </c>
@@ -2665,13 +2993,13 @@
         <v>132</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>133</v>
       </c>
@@ -2685,10 +3013,10 @@
         <v>135</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>136</v>
       </c>
@@ -2702,10 +3030,10 @@
         <v>138</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>139</v>
       </c>
@@ -2719,10 +3047,10 @@
         <v>141</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>142</v>
       </c>
@@ -2730,16 +3058,16 @@
         <v>7</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>143</v>
       </c>
@@ -2750,13 +3078,13 @@
         <v>144</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>145</v>
       </c>
@@ -2770,10 +3098,10 @@
         <v>147</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>148</v>
       </c>
@@ -2787,10 +3115,10 @@
         <v>150</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>151</v>
       </c>
@@ -2804,10 +3132,10 @@
         <v>153</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>154</v>
       </c>
@@ -2821,10 +3149,10 @@
         <v>153</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>156</v>
       </c>
@@ -2835,13 +3163,13 @@
         <v>157</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>158</v>
       </c>
@@ -2855,10 +3183,10 @@
         <v>160</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>161</v>
       </c>
@@ -2869,10 +3197,13 @@
         <v>162</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>343</v>
+        <v>400</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2883,13 +3214,13 @@
         <v>7</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2900,13 +3231,13 @@
         <v>7</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2923,7 +3254,7 @@
         <v>167</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2931,7 +3262,7 @@
         <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>169</v>
@@ -2940,7 +3271,7 @@
         <v>170</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2957,7 +3288,7 @@
         <v>173</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2974,7 +3305,7 @@
         <v>176</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2991,7 +3322,7 @@
         <v>179</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3008,7 +3339,7 @@
         <v>182</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3025,7 +3356,7 @@
         <v>185</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3042,7 +3373,7 @@
         <v>188</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3059,7 +3390,7 @@
         <v>188</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3076,10 +3407,10 @@
         <v>193</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3096,7 +3427,7 @@
         <v>196</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3113,7 +3444,7 @@
         <v>199</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3127,10 +3458,10 @@
         <v>201</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3144,10 +3475,10 @@
         <v>203</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3161,10 +3492,10 @@
         <v>205</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3181,7 +3512,7 @@
         <v>208</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3198,7 +3529,7 @@
         <v>211</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3215,7 +3546,7 @@
         <v>91</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>319</v>
+        <v>404</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3232,7 +3563,7 @@
         <v>216</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3249,7 +3580,7 @@
         <v>208</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3266,7 +3597,7 @@
         <v>91</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3283,7 +3614,7 @@
         <v>223</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3300,7 +3631,7 @@
         <v>91</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>319</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3317,7 +3648,7 @@
         <v>223</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3334,7 +3665,7 @@
         <v>91</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3351,7 +3682,7 @@
         <v>223</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3359,7 +3690,7 @@
         <v>232</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>233</v>
@@ -3368,7 +3699,7 @@
         <v>91</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3379,14 +3710,14 @@
         <v>235</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="F94" s="8"/>
       <c r="G94" s="6" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3400,7 +3731,7 @@
         <v>237</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="F95" s="8"/>
     </row>
@@ -3427,22 +3758,22 @@
         <v>241</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="F97" s="8"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F98" s="8"/>
     </row>
@@ -3451,22 +3782,22 @@
         <v>242</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="F99" s="8"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>243</v>
@@ -3478,22 +3809,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>